<commit_message>
Added user groups changing functionality
</commit_message>
<xml_diff>
--- a/server/loadDataFromExcelToDb/data.xlsx
+++ b/server/loadDataFromExcelToDb/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\icyHorizonsDeploy\server\loadDataFromExcelToDb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B577EEB0-1B1F-4F72-BFEE-77B6973584CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622AB817-5AC9-42DF-BD1F-D57FA069A34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminCenters" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="Tours" sheetId="4" r:id="rId5"/>
     <sheet name="Markers" sheetId="6" r:id="rId6"/>
     <sheet name="Roles" sheetId="7" r:id="rId7"/>
+    <sheet name="userGroupAnalysis" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="246">
   <si>
     <t>name</t>
   </si>
@@ -732,6 +733,45 @@
   </si>
   <si>
     <t>3083523.00</t>
+  </si>
+  <si>
+    <t>Экотуристы</t>
+  </si>
+  <si>
+    <t>Любитель природы</t>
+  </si>
+  <si>
+    <t>Охотник за адреналином</t>
+  </si>
+  <si>
+    <t>Исследователь культур</t>
+  </si>
+  <si>
+    <t>Ценитель отдыха</t>
+  </si>
+  <si>
+    <t>Экстремальные туристы</t>
+  </si>
+  <si>
+    <t>Этнографические туристы</t>
+  </si>
+  <si>
+    <t>Рекреационные туристы</t>
+  </si>
+  <si>
+    <t>Путешествуете ради экологии и живописных мест</t>
+  </si>
+  <si>
+    <t>Ищете драйв, экстрим и новые высоты</t>
+  </si>
+  <si>
+    <t>Углубляетесь в традиции и быт народов</t>
+  </si>
+  <si>
+    <t>Наслаждаетесь комфортом, спокойствием и природой</t>
+  </si>
+  <si>
+    <t>nameForUser</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1187,7 @@
   </sheetPr>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3166,4 +3206,79 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C1E2B9-39BE-45EC-AFB0-C4686DAD09EE}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>